<commit_message>
Update Para Meteric sce
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Par-B_RSD_HLI.xlsx
+++ b/SuppXLS/Scen_Par-B_RSD_HLI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97EC2AF-122F-4832-8F3B-0FD01C529157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F45BA2-821C-426E-B3F7-821DF5B660EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -719,7 +719,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1235,15 +1235,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1258,12 +1249,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="14" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1276,8 +1261,23 @@
     <xf numFmtId="1" fontId="3" fillId="14" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="15" fillId="9" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="15" fillId="9" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Good" xfId="3" builtinId="26"/>
@@ -2444,12 +2444,12 @@
       <c r="Z15" s="20"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -2533,11 +2533,11 @@
       <c r="A19" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
       <c r="G19" s="28"/>
@@ -2565,11 +2565,11 @@
       <c r="A20" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
       <c r="G20" s="28"/>
@@ -2657,11 +2657,11 @@
       <c r="A23" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
@@ -2745,11 +2745,11 @@
       <c r="A26" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
@@ -2863,11 +2863,11 @@
       <c r="A30" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
       <c r="G30" s="20"/>
@@ -2895,11 +2895,11 @@
       <c r="A31" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
       <c r="G31" s="20"/>
@@ -8597,10 +8597,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="38" t="s">
         <v>157</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -8608,10 +8608,10 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42">
+      <c r="B3" s="39">
         <v>1</v>
       </c>
-      <c r="C3" s="43" t="str">
+      <c r="C3" s="40" t="str">
         <f>Scenarios!$M$18&amp; E3</f>
         <v>Constrain share of HPs at HLI 2</v>
       </c>
@@ -8620,10 +8620,10 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="42">
+      <c r="B4" s="39">
         <v>2</v>
       </c>
-      <c r="C4" s="43" t="str">
+      <c r="C4" s="40" t="str">
         <f>Scenarios!$M$18&amp; E4</f>
         <v>Constrain share of HPs at HLI 2.3</v>
       </c>
@@ -8632,11 +8632,11 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="42">
+      <c r="B5" s="39">
         <f>B4+1</f>
         <v>3</v>
       </c>
-      <c r="C5" s="43" t="str">
+      <c r="C5" s="40" t="str">
         <f>Scenarios!$M$18&amp; E5</f>
         <v>Constrain share of HPs at HLI 2.5</v>
       </c>
@@ -8645,11 +8645,11 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="42">
+      <c r="B6" s="39">
         <f t="shared" ref="B6:B9" si="0">B5+1</f>
         <v>4</v>
       </c>
-      <c r="C6" s="43" t="str">
+      <c r="C6" s="40" t="str">
         <f>Scenarios!$M$18&amp; E6</f>
         <v>Constrain share of HPs at HLI 3</v>
       </c>
@@ -8658,11 +8658,11 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="42">
+      <c r="B7" s="39">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="43" t="str">
+      <c r="C7" s="40" t="str">
         <f>Scenarios!$M$18&amp; E7</f>
         <v>Constrain share of HPs at HLI 3.5</v>
       </c>
@@ -8671,11 +8671,11 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="42">
+      <c r="B8" s="39">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="43" t="str">
+      <c r="C8" s="40" t="str">
         <f>Scenarios!$M$18&amp; E8</f>
         <v>Constrain share of HPs at HLI 4</v>
       </c>
@@ -8684,11 +8684,11 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="42">
+      <c r="B9" s="39">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="43" t="str">
+      <c r="C9" s="40" t="str">
         <f>Scenarios!$M$18&amp; E9</f>
         <v>Constrain share of HPs at HLI 4.5</v>
       </c>
@@ -8706,7 +8706,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8724,7 +8724,7 @@
       </c>
     </row>
     <row r="2" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44">
+      <c r="A2" s="41">
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -8831,7 +8831,7 @@
       </c>
     </row>
     <row r="4" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="42" t="s">
         <v>160</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -8895,114 +8895,114 @@
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="AA4" s="8"/>
-      <c r="AB4" s="46" t="s">
+      <c r="AB4" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="AC4" s="47"/>
-      <c r="AD4" s="47"/>
-      <c r="AE4" s="47"/>
-      <c r="AF4" s="47"/>
-      <c r="AG4" s="47"/>
-      <c r="AH4" s="47"/>
-      <c r="AI4" s="47"/>
+      <c r="AC4" s="53"/>
+      <c r="AD4" s="53"/>
+      <c r="AE4" s="53"/>
+      <c r="AF4" s="53"/>
+      <c r="AG4" s="53"/>
+      <c r="AH4" s="53"/>
+      <c r="AI4" s="53"/>
       <c r="AJ4" s="8"/>
-      <c r="AK4" s="47" t="s">
+      <c r="AK4" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="AL4" s="47"/>
-      <c r="AM4" s="47"/>
-      <c r="AN4" s="47"/>
-      <c r="AO4" s="47"/>
-      <c r="AP4" s="47"/>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="47"/>
-      <c r="AS4" s="47"/>
+      <c r="AL4" s="53"/>
+      <c r="AM4" s="53"/>
+      <c r="AN4" s="53"/>
+      <c r="AO4" s="53"/>
+      <c r="AP4" s="53"/>
+      <c r="AQ4" s="53"/>
+      <c r="AR4" s="53"/>
+      <c r="AS4" s="53"/>
       <c r="AT4" s="8"/>
-      <c r="AU4" s="46" t="s">
+      <c r="AU4" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="AV4" s="47"/>
-      <c r="AW4" s="47"/>
-      <c r="AX4" s="47"/>
-      <c r="AY4" s="47"/>
-      <c r="AZ4" s="47"/>
-      <c r="BA4" s="47"/>
-      <c r="BB4" s="47"/>
-      <c r="BC4" s="47"/>
+      <c r="AV4" s="53"/>
+      <c r="AW4" s="53"/>
+      <c r="AX4" s="53"/>
+      <c r="AY4" s="53"/>
+      <c r="AZ4" s="53"/>
+      <c r="BA4" s="53"/>
+      <c r="BB4" s="53"/>
+      <c r="BC4" s="53"/>
     </row>
     <row r="5" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="45">
+      <c r="B5" s="42">
         <v>1</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="47">
         <f>INDEX($AB$6:$AI$14, MATCH(C13, $AA$6:$AA$14, 0), MATCH($V$5, $AB$3:$AI$3, 0))</f>
         <v>0.76682617615099935</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="47">
         <f t="shared" ref="D5:H5" si="0">INDEX($AB$6:$AI$14, MATCH(D13, $AA$6:$AA$14, 0), MATCH($V$5, $AB$3:$AI$3, 0))</f>
         <v>0.5138907043261417</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="47">
         <f t="shared" si="0"/>
         <v>0.37584533679027893</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="47">
         <f t="shared" si="0"/>
         <v>0.16552806134367962</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="47">
         <f t="shared" si="0"/>
         <v>9.1492186931267622E-2</v>
       </c>
-      <c r="H5" s="52">
+      <c r="H5" s="47">
         <f t="shared" si="0"/>
         <v>3.6630747396996691E-2</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="47">
         <f>INDEX($AL$6:$AS$14, MATCH($I13, $AK$6:$AK$14, 0), MATCH($V5, $AL$3:$AS$3, 0))</f>
         <v>0.48602123970467664</v>
       </c>
-      <c r="J5" s="52">
+      <c r="J5" s="47">
         <f t="shared" ref="J5:N5" si="1">INDEX($AL$6:$AS$14, MATCH(J13, $AK$6:$AK$14, 0), MATCH($V$5, $AL$3:$AS$3, 0))</f>
         <v>0.25380085256173046</v>
       </c>
-      <c r="K5" s="52">
+      <c r="K5" s="47">
         <f t="shared" si="1"/>
         <v>8.9754023843298891E-2</v>
       </c>
-      <c r="L5" s="52">
+      <c r="L5" s="47">
         <f t="shared" si="1"/>
         <v>5.0511604601422351E-2</v>
       </c>
-      <c r="M5" s="52">
+      <c r="M5" s="47">
         <f t="shared" si="1"/>
         <v>3.2210497290905374E-2</v>
       </c>
-      <c r="N5" s="52">
+      <c r="N5" s="47">
         <f t="shared" si="1"/>
         <v>3.054309712927282E-2</v>
       </c>
-      <c r="O5" s="52">
+      <c r="O5" s="47">
         <f>INDEX($AV$6:$BC$14, MATCH(O13, $AU$6:$AU$14, 0), MATCH($V5, $AV$3:$BC$3, 0))</f>
         <v>0.14983014442834014</v>
       </c>
-      <c r="P5" s="52">
+      <c r="P5" s="47">
         <f t="shared" ref="P5:T5" si="2">INDEX($AV$6:$BC$14, MATCH(P13, $AU$6:$AU$14, 0), MATCH($V5, $AV$3:$BC$3, 0))</f>
         <v>6.6011404930960929E-2</v>
       </c>
-      <c r="Q5" s="52">
+      <c r="Q5" s="47">
         <f t="shared" si="2"/>
         <v>5.6979596817344061E-2</v>
       </c>
-      <c r="R5" s="52">
+      <c r="R5" s="47">
         <f t="shared" si="2"/>
         <v>2.8856450394145666E-2</v>
       </c>
-      <c r="S5" s="52">
+      <c r="S5" s="47">
         <f t="shared" si="2"/>
         <v>7.3325429420576533E-3</v>
       </c>
-      <c r="T5" s="52">
+      <c r="T5" s="47">
         <f t="shared" si="2"/>
         <v>3.2086171243230267E-3</v>
       </c>
@@ -9012,156 +9012,156 @@
       </c>
       <c r="W5" s="8"/>
       <c r="AA5" s="8"/>
-      <c r="AB5" s="48" t="s">
+      <c r="AB5" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="AC5" s="49" t="s">
+      <c r="AC5" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="AD5" s="50" t="s">
+      <c r="AD5" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="AE5" s="49" t="s">
+      <c r="AE5" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="AF5" s="49" t="s">
+      <c r="AF5" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="AG5" s="49" t="s">
+      <c r="AG5" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="AH5" s="49" t="s">
+      <c r="AH5" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="AI5" s="49" t="s">
+      <c r="AI5" s="44" t="s">
         <v>173</v>
       </c>
       <c r="AJ5" s="8"/>
       <c r="AK5" s="8"/>
-      <c r="AL5" s="48" t="s">
+      <c r="AL5" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="AM5" s="49" t="s">
+      <c r="AM5" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="AN5" s="50" t="s">
+      <c r="AN5" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="AO5" s="49" t="s">
+      <c r="AO5" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="AP5" s="49" t="s">
+      <c r="AP5" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="AQ5" s="49" t="s">
+      <c r="AQ5" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="AR5" s="49" t="s">
+      <c r="AR5" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="AS5" s="49" t="s">
+      <c r="AS5" s="44" t="s">
         <v>173</v>
       </c>
       <c r="AT5" s="8"/>
       <c r="AU5" s="8"/>
-      <c r="AV5" s="48" t="s">
+      <c r="AV5" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="AW5" s="49" t="s">
+      <c r="AW5" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="AX5" s="50" t="s">
+      <c r="AX5" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="AY5" s="49" t="s">
+      <c r="AY5" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="AZ5" s="49" t="s">
+      <c r="AZ5" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="BA5" s="49" t="s">
+      <c r="BA5" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="BB5" s="49" t="s">
+      <c r="BB5" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="BC5" s="49" t="s">
+      <c r="BC5" s="44" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B6" s="45">
+      <c r="B6" s="42">
         <v>2</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="47">
         <f>INDEX($AB$6:$AI$14, MATCH(C13, $AA$6:$AA$14, 0), MATCH($V$6, $AB$3:$AI$3, 0))</f>
         <v>0.95418880111755022</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="47">
         <f t="shared" ref="D6:H6" si="3">INDEX($AB$6:$AI$14, MATCH(D13, $AA$6:$AA$14, 0), MATCH($V$6, $AB$3:$AI$3, 0))</f>
         <v>0.70275414783970647</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="47">
         <f t="shared" si="3"/>
         <v>0.51506861469064869</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="47">
         <f t="shared" si="3"/>
         <v>0.29053559209062707</v>
       </c>
-      <c r="G6" s="52">
+      <c r="G6" s="47">
         <f t="shared" si="3"/>
         <v>0.15300882371326033</v>
       </c>
-      <c r="H6" s="52">
+      <c r="H6" s="47">
         <f t="shared" si="3"/>
         <v>5.4970533940220757E-2</v>
       </c>
-      <c r="I6" s="52">
+      <c r="I6" s="47">
         <f>INDEX($AL$6:$AS$14, MATCH(I13, $AK$6:$AK$14, 0), MATCH($V6, $AL$3:$AS$3, 0))</f>
         <v>0.74725860659793841</v>
       </c>
-      <c r="J6" s="52">
+      <c r="J6" s="47">
         <f t="shared" ref="J6:N6" si="4">INDEX($AL$6:$AS$14, MATCH(J13, $AK$6:$AK$14, 0), MATCH($V6, $AL$3:$AS$3, 0))</f>
         <v>0.48042786872418958</v>
       </c>
-      <c r="K6" s="52">
+      <c r="K6" s="47">
         <f t="shared" si="4"/>
         <v>0.19240027281705166</v>
       </c>
-      <c r="L6" s="52">
+      <c r="L6" s="47">
         <f t="shared" si="4"/>
         <v>9.4333345509310967E-2</v>
       </c>
-      <c r="M6" s="52">
+      <c r="M6" s="47">
         <f t="shared" si="4"/>
         <v>5.6332486553475364E-2</v>
       </c>
-      <c r="N6" s="52">
+      <c r="N6" s="47">
         <f t="shared" si="4"/>
         <v>4.54767509141593E-2</v>
       </c>
-      <c r="O6" s="52">
+      <c r="O6" s="47">
         <f>INDEX($AV$6:$BC$14, MATCH(O13, $AU$6:$AU$14, 0), MATCH($V6, $AV$3:$BC$3, 0))</f>
         <v>0.49056643348839696</v>
       </c>
-      <c r="P6" s="52">
+      <c r="P6" s="47">
         <f t="shared" ref="P6:T6" si="5">INDEX($AV$6:$BC$14, MATCH(P13, $AU$6:$AU$14, 0), MATCH($V6, $AV$3:$BC$3, 0))</f>
         <v>0.22200714259760385</v>
       </c>
-      <c r="Q6" s="52">
+      <c r="Q6" s="47">
         <f t="shared" si="5"/>
         <v>0.12698439253107691</v>
       </c>
-      <c r="R6" s="52">
+      <c r="R6" s="47">
         <f t="shared" si="5"/>
         <v>5.7199757058308189E-2</v>
       </c>
-      <c r="S6" s="52">
+      <c r="S6" s="47">
         <f t="shared" si="5"/>
         <v>1.5850994164039133E-2</v>
       </c>
-      <c r="T6" s="52">
+      <c r="T6" s="47">
         <f t="shared" si="5"/>
         <v>5.8437278169573741E-3</v>
       </c>
@@ -9170,163 +9170,163 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W6" s="8"/>
-      <c r="AA6" s="48" t="s">
+      <c r="AA6" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="AB6" s="52">
+      <c r="AB6" s="47">
         <v>0.99986614214614677</v>
       </c>
-      <c r="AC6" s="52">
+      <c r="AC6" s="47">
         <v>0.99999895018069218</v>
       </c>
-      <c r="AD6" s="52">
+      <c r="AD6" s="47">
         <v>0.99999997827100517</v>
       </c>
-      <c r="AE6" s="52">
+      <c r="AE6" s="47">
         <v>0.99999999999986411</v>
       </c>
-      <c r="AF6" s="52">
+      <c r="AF6" s="47">
         <v>1</v>
       </c>
-      <c r="AG6" s="52">
+      <c r="AG6" s="47">
         <v>1</v>
       </c>
-      <c r="AH6" s="52">
+      <c r="AH6" s="47">
         <v>1</v>
       </c>
-      <c r="AI6" s="52">
+      <c r="AI6" s="47">
         <v>0</v>
       </c>
       <c r="AJ6" s="8"/>
-      <c r="AK6" s="48" t="s">
+      <c r="AK6" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="AL6" s="52">
+      <c r="AL6" s="47">
         <v>0.99358230344905218</v>
       </c>
-      <c r="AM6" s="52">
+      <c r="AM6" s="47">
         <v>0.99961797061500135</v>
       </c>
-      <c r="AN6" s="52">
+      <c r="AN6" s="47">
         <v>0.99996097211163748</v>
       </c>
-      <c r="AO6" s="52">
+      <c r="AO6" s="47">
         <v>0.99999996888648002</v>
       </c>
-      <c r="AP6" s="52">
+      <c r="AP6" s="47">
         <v>0.9999999999968846</v>
       </c>
-      <c r="AQ6" s="52">
+      <c r="AQ6" s="47">
         <v>1</v>
       </c>
-      <c r="AR6" s="52">
+      <c r="AR6" s="47">
         <v>1</v>
       </c>
-      <c r="AS6" s="52">
+      <c r="AS6" s="47">
         <v>0</v>
       </c>
       <c r="AT6" s="8"/>
-      <c r="AU6" s="48" t="s">
+      <c r="AU6" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="AV6" s="52">
+      <c r="AV6" s="47">
         <v>0.99867076285153633</v>
       </c>
-      <c r="AW6" s="52">
+      <c r="AW6" s="47">
         <v>0.99999490602709384</v>
       </c>
-      <c r="AX6" s="52">
+      <c r="AX6" s="47">
         <v>0.99999995653338158</v>
       </c>
-      <c r="AY6" s="52">
+      <c r="AY6" s="47">
         <v>0.99999999999999312</v>
       </c>
-      <c r="AZ6" s="52">
+      <c r="AZ6" s="47">
         <v>1</v>
       </c>
-      <c r="BA6" s="52">
+      <c r="BA6" s="47">
         <v>1</v>
       </c>
-      <c r="BB6" s="52">
+      <c r="BB6" s="47">
         <v>1</v>
       </c>
-      <c r="BC6" s="52">
+      <c r="BC6" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B7" s="45">
+      <c r="B7" s="42">
         <v>3</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="47">
         <f>INDEX($AB$6:$AI$14, MATCH(C13, $AA$6:$AA$14, 0), MATCH($V$7, $AB$3:$AI$3, 0))</f>
         <v>0.98998748585906793</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="47">
         <f t="shared" ref="D7:H7" si="6">INDEX($AB$6:$AI$14, MATCH(D13, $AA$6:$AA$14, 0), MATCH($V$7, $AB$3:$AI$3, 0))</f>
         <v>0.80620969874302539</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="47">
         <f t="shared" si="6"/>
         <v>0.60792230376456446</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="47">
         <f t="shared" si="6"/>
         <v>0.39292301197938029</v>
       </c>
-      <c r="G7" s="52">
+      <c r="G7" s="47">
         <f t="shared" si="6"/>
         <v>0.20660004501142309</v>
       </c>
-      <c r="H7" s="52">
+      <c r="H7" s="47">
         <f t="shared" si="6"/>
         <v>7.0785662206478708E-2</v>
       </c>
-      <c r="I7" s="52">
+      <c r="I7" s="47">
         <f>INDEX($AL$6:$AS$14, MATCH(I13, $AK$6:$AK$14, 0), MATCH($V7, $AL$3:$AS$3, 0))</f>
         <v>0.87143015426775872</v>
       </c>
-      <c r="J7" s="52">
+      <c r="J7" s="47">
         <f t="shared" ref="J7:N7" si="7">INDEX($AL$6:$AS$14, MATCH(J13, $AK$6:$AK$14, 0), MATCH($V7, $AL$3:$AS$3, 0))</f>
         <v>0.64054584703308814</v>
       </c>
-      <c r="K7" s="52">
+      <c r="K7" s="47">
         <f t="shared" si="7"/>
         <v>0.28991681177663592</v>
       </c>
-      <c r="L7" s="52">
+      <c r="L7" s="47">
         <f t="shared" si="7"/>
         <v>0.13618656405660809</v>
       </c>
-      <c r="M7" s="52">
+      <c r="M7" s="47">
         <f t="shared" si="7"/>
         <v>7.9115975834815E-2</v>
       </c>
-      <c r="N7" s="52">
+      <c r="N7" s="47">
         <f t="shared" si="7"/>
         <v>5.8354873920238394E-2</v>
       </c>
-      <c r="O7" s="52">
+      <c r="O7" s="47">
         <f>INDEX($AV$6:$BC$14, MATCH(O13, $AU$6:$AU$14, 0), MATCH($V7, $AV$3:$BC$3, 0))</f>
         <v>0.74280813134921952</v>
       </c>
-      <c r="P7" s="52">
+      <c r="P7" s="47">
         <f t="shared" ref="P7:T7" si="8">INDEX($AV$6:$BC$14, MATCH(P13, $AU$6:$AU$14, 0), MATCH($V7, $AV$3:$BC$3, 0))</f>
         <v>0.39296290098211079</v>
       </c>
-      <c r="Q7" s="52">
+      <c r="Q7" s="47">
         <f t="shared" si="8"/>
         <v>0.19835620119859471</v>
       </c>
-      <c r="R7" s="52">
+      <c r="R7" s="47">
         <f t="shared" si="8"/>
         <v>8.5976160021217857E-2</v>
       </c>
-      <c r="S7" s="52">
+      <c r="S7" s="47">
         <f t="shared" si="8"/>
         <v>2.5396980814932565E-2</v>
       </c>
-      <c r="T7" s="52">
+      <c r="T7" s="47">
         <f t="shared" si="8"/>
         <v>8.5326893308700167E-3</v>
       </c>
@@ -9335,163 +9335,163 @@
         <v>2.5</v>
       </c>
       <c r="W7" s="8"/>
-      <c r="AA7" s="49" t="s">
+      <c r="AA7" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="AB7" s="52">
+      <c r="AB7" s="47">
         <v>0.96885301500182108</v>
       </c>
-      <c r="AC7" s="52">
+      <c r="AC7" s="47">
         <v>0.99736560266376562</v>
       </c>
-      <c r="AD7" s="52">
+      <c r="AD7" s="47">
         <v>0.99967208422117826</v>
       </c>
-      <c r="AE7" s="52">
+      <c r="AE7" s="47">
         <v>0.99999963010770987</v>
       </c>
-      <c r="AF7" s="52">
+      <c r="AF7" s="47">
         <v>0.99999999995815858</v>
       </c>
-      <c r="AG7" s="52">
+      <c r="AG7" s="47">
         <v>0.99999999999999956</v>
       </c>
-      <c r="AH7" s="52">
+      <c r="AH7" s="47">
         <v>1</v>
       </c>
-      <c r="AI7" s="52">
+      <c r="AI7" s="47">
         <v>0</v>
       </c>
       <c r="AJ7" s="8"/>
-      <c r="AK7" s="49" t="s">
+      <c r="AK7" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="AL7" s="52">
+      <c r="AL7" s="47">
         <v>0.7694627396275191</v>
       </c>
-      <c r="AM7" s="52">
+      <c r="AM7" s="47">
         <v>0.92091247414921895</v>
       </c>
-      <c r="AN7" s="52">
+      <c r="AN7" s="47">
         <v>0.96860489728090593</v>
       </c>
-      <c r="AO7" s="52">
+      <c r="AO7" s="47">
         <v>0.99857871934570608</v>
       </c>
-      <c r="AP7" s="52">
+      <c r="AP7" s="47">
         <v>0.99998003334500252</v>
       </c>
-      <c r="AQ7" s="52">
+      <c r="AQ7" s="47">
         <v>0.99999991591209203</v>
       </c>
-      <c r="AR7" s="52">
+      <c r="AR7" s="47">
         <v>0.99999999989582478</v>
       </c>
-      <c r="AS7" s="52">
+      <c r="AS7" s="47">
         <v>0</v>
       </c>
       <c r="AT7" s="8"/>
-      <c r="AU7" s="49" t="s">
+      <c r="AU7" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="AV7" s="52">
+      <c r="AV7" s="47">
         <v>0.6130931526036395</v>
       </c>
-      <c r="AW7" s="52">
+      <c r="AW7" s="47">
         <v>0.87842619586393023</v>
       </c>
-      <c r="AX7" s="52">
+      <c r="AX7" s="47">
         <v>0.9602560960127382</v>
       </c>
-      <c r="AY7" s="52">
+      <c r="AY7" s="47">
         <v>0.99935891586967851</v>
       </c>
-      <c r="AZ7" s="52">
+      <c r="AZ7" s="47">
         <v>0.99999860849411715</v>
       </c>
-      <c r="BA7" s="52">
+      <c r="BA7" s="47">
         <v>0.99999999961862751</v>
       </c>
-      <c r="BB7" s="52">
+      <c r="BB7" s="47">
         <v>0.99999999999998723</v>
       </c>
-      <c r="BC7" s="52">
+      <c r="BC7" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B8" s="45">
+      <c r="B8" s="42">
         <v>4</v>
       </c>
-      <c r="C8" s="52">
+      <c r="C8" s="47">
         <f>INDEX($AB$6:$AI$14, MATCH(C13, $AA$6:$AA$14, 0), MATCH($V$8, $AB$3:$AI$3, 0))</f>
         <v>0.99995633197497646</v>
       </c>
-      <c r="D8" s="52">
+      <c r="D8" s="47">
         <f t="shared" ref="D8:H8" si="9">INDEX($AB$6:$AI$14, MATCH(D13, $AA$6:$AA$14, 0), MATCH($V$8, $AB$3:$AI$3, 0))</f>
         <v>0.95479136080813631</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="47">
         <f t="shared" si="9"/>
         <v>0.80626831138166599</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="47">
         <f t="shared" si="9"/>
         <v>0.66588242910237538</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="47">
         <f t="shared" si="9"/>
         <v>0.38021044483571315</v>
       </c>
-      <c r="H8" s="52">
+      <c r="H8" s="47">
         <f t="shared" si="9"/>
         <v>0.12533343317165579</v>
       </c>
-      <c r="I8" s="52">
+      <c r="I8" s="47">
         <f>INDEX($AL$6:$AS$14, MATCH(I13, $AK$6:$AK$14, 0), MATCH($V8, $AL$3:$AS$3, 0))</f>
         <v>0.98931553681492335</v>
       </c>
-      <c r="J8" s="52">
+      <c r="J8" s="47">
         <f t="shared" ref="J8:N8" si="10">INDEX($AL$6:$AS$14, MATCH(J13, $AK$6:$AK$14, 0), MATCH($V8, $AL$3:$AS$3, 0))</f>
         <v>0.91657755012121211</v>
       </c>
-      <c r="K8" s="52">
+      <c r="K8" s="47">
         <f t="shared" si="10"/>
         <v>0.59290175446950721</v>
       </c>
-      <c r="L8" s="52">
+      <c r="L8" s="47">
         <f t="shared" si="10"/>
         <v>0.28933976981199794</v>
       </c>
-      <c r="M8" s="52">
+      <c r="M8" s="47">
         <f t="shared" si="10"/>
         <v>0.16531868864588461</v>
       </c>
-      <c r="N8" s="52">
+      <c r="N8" s="47">
         <f t="shared" si="10"/>
         <v>0.10300763832828137</v>
       </c>
-      <c r="O8" s="52">
+      <c r="O8" s="47">
         <f>INDEX($AV$6:$BC$14, MATCH(O13, $AU$6:$AU$14, 0), MATCH($V8, $AV$3:$BC$3, 0))</f>
         <v>0.9903894839477374</v>
       </c>
-      <c r="P8" s="52">
+      <c r="P8" s="47">
         <f t="shared" ref="P8:T8" si="11">INDEX($AV$6:$BC$14, MATCH(P13, $AU$6:$AU$14, 0), MATCH($V8, $AV$3:$BC$3, 0))</f>
         <v>0.83221694488457221</v>
       </c>
-      <c r="Q8" s="52">
+      <c r="Q8" s="47">
         <f t="shared" si="11"/>
         <v>0.45447244481580307</v>
       </c>
-      <c r="R8" s="52">
+      <c r="R8" s="47">
         <f t="shared" si="11"/>
         <v>0.20212850255165354</v>
       </c>
-      <c r="S8" s="52">
+      <c r="S8" s="47">
         <f t="shared" si="11"/>
         <v>7.1339545297204487E-2</v>
       </c>
-      <c r="T8" s="52">
+      <c r="T8" s="47">
         <f t="shared" si="11"/>
         <v>2.0430952713542849E-2</v>
       </c>
@@ -9500,163 +9500,163 @@
         <v>3</v>
       </c>
       <c r="W8" s="8"/>
-      <c r="AA8" s="50" t="s">
+      <c r="AA8" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="AB8" s="52">
+      <c r="AB8" s="47">
         <v>0.93969745300565943</v>
       </c>
-      <c r="AC8" s="52">
+      <c r="AC8" s="47">
         <v>0.99622594121059427</v>
       </c>
-      <c r="AD8" s="52">
+      <c r="AD8" s="47">
         <v>0.99968448066910742</v>
       </c>
-      <c r="AE8" s="52">
+      <c r="AE8" s="47">
         <v>0.99999993665897058</v>
       </c>
-      <c r="AF8" s="52">
+      <c r="AF8" s="47">
         <v>0.99999999999956379</v>
       </c>
-      <c r="AG8" s="52">
+      <c r="AG8" s="47">
         <v>1</v>
       </c>
-      <c r="AH8" s="52">
+      <c r="AH8" s="47">
         <v>1</v>
       </c>
-      <c r="AI8" s="52">
+      <c r="AI8" s="47">
         <v>0</v>
       </c>
       <c r="AJ8" s="8"/>
-      <c r="AK8" s="50" t="s">
+      <c r="AK8" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="AL8" s="52">
+      <c r="AL8" s="47">
         <v>0.63358245624321075</v>
       </c>
-      <c r="AM8" s="52">
+      <c r="AM8" s="47">
         <v>0.84081469035187228</v>
       </c>
-      <c r="AN8" s="52">
+      <c r="AN8" s="47">
         <v>0.92442034414706997</v>
       </c>
-      <c r="AO8" s="52">
+      <c r="AO8" s="47">
         <v>0.99428940010152511</v>
       </c>
-      <c r="AP8" s="52">
+      <c r="AP8" s="47">
         <v>0.99985475279512115</v>
       </c>
-      <c r="AQ8" s="52">
+      <c r="AQ8" s="47">
         <v>0.99999880751297388</v>
       </c>
-      <c r="AR8" s="52">
+      <c r="AR8" s="47">
         <v>0.99999999691006625</v>
       </c>
-      <c r="AS8" s="52">
+      <c r="AS8" s="47">
         <v>0</v>
       </c>
       <c r="AT8" s="8"/>
-      <c r="AU8" s="50" t="s">
+      <c r="AU8" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="AV8" s="52">
+      <c r="AV8" s="47">
         <v>0.34194299028735675</v>
       </c>
-      <c r="AW8" s="52">
+      <c r="AW8" s="47">
         <v>0.71567219724569331</v>
       </c>
-      <c r="AX8" s="52">
+      <c r="AX8" s="47">
         <v>0.88905130905570107</v>
       </c>
-      <c r="AY8" s="52">
+      <c r="AY8" s="47">
         <v>0.99781515762844886</v>
       </c>
-      <c r="AZ8" s="52">
+      <c r="AZ8" s="47">
         <v>0.99999624728992065</v>
       </c>
-      <c r="BA8" s="52">
+      <c r="BA8" s="47">
         <v>0.99999999949395513</v>
       </c>
-      <c r="BB8" s="52">
+      <c r="BB8" s="47">
         <v>0.99999999999999489</v>
       </c>
-      <c r="BC8" s="52">
+      <c r="BC8" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B9" s="45">
+      <c r="B9" s="42">
         <v>5</v>
       </c>
-      <c r="C9" s="52">
+      <c r="C9" s="47">
         <f>INDEX($AB$6:$AI$14, MATCH(C13, $AA$6:$AA$14, 0), MATCH($V$9, $AB$3:$AI$3, 0))</f>
         <v>0.99999998312382343</v>
       </c>
-      <c r="D9" s="52">
+      <c r="D9" s="47">
         <f t="shared" ref="D9:H9" si="12">INDEX($AB$6:$AI$14, MATCH(D13, $AA$6:$AA$14, 0), MATCH($V$9, $AB$3:$AI$3, 0))</f>
         <v>0.99417194789886376</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="47">
         <f t="shared" si="12"/>
         <v>0.92710242952401201</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="47">
         <f t="shared" si="12"/>
         <v>0.87051976694100974</v>
       </c>
-      <c r="G9" s="52">
+      <c r="G9" s="47">
         <f t="shared" si="12"/>
         <v>0.58254904641534866</v>
       </c>
-      <c r="H9" s="52">
+      <c r="H9" s="47">
         <f t="shared" si="12"/>
         <v>0.20397754353748057</v>
       </c>
-      <c r="I9" s="52">
+      <c r="I9" s="47">
         <f>INDEX($AL$6:$AS$14, MATCH(I13, $AK$6:$AK$14, 0), MATCH($V9, $AL$3:$AS$3, 0))</f>
         <v>0.99973940839121955</v>
       </c>
-      <c r="J9" s="52">
+      <c r="J9" s="47">
         <f t="shared" ref="J9:N9" si="13">INDEX($AL$6:$AS$14, MATCH(J13, $AK$6:$AK$14, 0), MATCH($V9, $AL$3:$AS$3, 0))</f>
         <v>0.99191173064402915</v>
       </c>
-      <c r="K9" s="52">
+      <c r="K9" s="47">
         <f t="shared" si="13"/>
         <v>0.8470018886690438</v>
       </c>
-      <c r="L9" s="52">
+      <c r="L9" s="47">
         <f t="shared" si="13"/>
         <v>0.49480783925100147</v>
       </c>
-      <c r="M9" s="52">
+      <c r="M9" s="47">
         <f t="shared" si="13"/>
         <v>0.29645675583092174</v>
       </c>
-      <c r="N9" s="52">
+      <c r="N9" s="47">
         <f t="shared" si="13"/>
         <v>0.16841130134712209</v>
       </c>
-      <c r="O9" s="52">
+      <c r="O9" s="47">
         <f>INDEX($AV$6:$BC$14, MATCH(O13, $AU$6:$AU$14, 0), MATCH($V9, $AV$3:$BC$3, 0))</f>
         <v>0.99997215963294783</v>
       </c>
-      <c r="P9" s="52">
+      <c r="P9" s="47">
         <f t="shared" ref="P9:T9" si="14">INDEX($AV$6:$BC$14, MATCH(P13, $AU$6:$AU$14, 0), MATCH($V9, $AV$3:$BC$3, 0))</f>
         <v>0.98600872265415918</v>
       </c>
-      <c r="Q9" s="52">
+      <c r="Q9" s="47">
         <f t="shared" si="14"/>
         <v>0.73196550526672355</v>
       </c>
-      <c r="R9" s="52">
+      <c r="R9" s="47">
         <f t="shared" si="14"/>
         <v>0.38127737390844418</v>
       </c>
-      <c r="S9" s="52">
+      <c r="S9" s="47">
         <f t="shared" si="14"/>
         <v>0.16389933245411942</v>
       </c>
-      <c r="T9" s="52">
+      <c r="T9" s="47">
         <f t="shared" si="14"/>
         <v>4.4138172035112347E-2</v>
       </c>
@@ -9665,163 +9665,163 @@
         <v>3.5</v>
       </c>
       <c r="W9" s="8"/>
-      <c r="AA9" s="49" t="s">
+      <c r="AA9" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="AB9" s="52">
+      <c r="AB9" s="47">
         <v>0.76682617615099935</v>
       </c>
-      <c r="AC9" s="52">
+      <c r="AC9" s="47">
         <v>0.95418880111755022</v>
       </c>
-      <c r="AD9" s="52">
+      <c r="AD9" s="47">
         <v>0.98998748585906793</v>
       </c>
-      <c r="AE9" s="52">
+      <c r="AE9" s="47">
         <v>0.99995633197497646</v>
       </c>
-      <c r="AF9" s="52">
+      <c r="AF9" s="47">
         <v>0.99999998312382343</v>
       </c>
-      <c r="AG9" s="52">
+      <c r="AG9" s="47">
         <v>0.99999999999945333</v>
       </c>
-      <c r="AH9" s="52">
+      <c r="AH9" s="47">
         <v>1</v>
       </c>
-      <c r="AI9" s="52">
+      <c r="AI9" s="47">
         <v>0</v>
       </c>
       <c r="AJ9" s="8"/>
-      <c r="AK9" s="49" t="s">
+      <c r="AK9" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="AL9" s="52">
+      <c r="AL9" s="47">
         <v>0.48602123970467664</v>
       </c>
-      <c r="AM9" s="52">
+      <c r="AM9" s="47">
         <v>0.74725860659793841</v>
       </c>
-      <c r="AN9" s="52">
+      <c r="AN9" s="47">
         <v>0.87143015426775872</v>
       </c>
-      <c r="AO9" s="52">
+      <c r="AO9" s="47">
         <v>0.98931553681492335</v>
       </c>
-      <c r="AP9" s="52">
+      <c r="AP9" s="47">
         <v>0.99973940839121955</v>
       </c>
-      <c r="AQ9" s="52">
+      <c r="AQ9" s="47">
         <v>0.99999823974334678</v>
       </c>
-      <c r="AR9" s="52">
+      <c r="AR9" s="47">
         <v>0.99999999680227936</v>
       </c>
-      <c r="AS9" s="52">
+      <c r="AS9" s="47">
         <v>0</v>
       </c>
       <c r="AT9" s="8"/>
-      <c r="AU9" s="49" t="s">
+      <c r="AU9" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="AV9" s="52">
+      <c r="AV9" s="47">
         <v>0.14983014442834014</v>
       </c>
-      <c r="AW9" s="52">
+      <c r="AW9" s="47">
         <v>0.49056643348839696</v>
       </c>
-      <c r="AX9" s="52">
+      <c r="AX9" s="47">
         <v>0.74280813134921952</v>
       </c>
-      <c r="AY9" s="52">
+      <c r="AY9" s="47">
         <v>0.9903894839477374</v>
       </c>
-      <c r="AZ9" s="52">
+      <c r="AZ9" s="47">
         <v>0.99997215963294783</v>
       </c>
-      <c r="BA9" s="52">
+      <c r="BA9" s="47">
         <v>0.99999999466107425</v>
       </c>
-      <c r="BB9" s="52">
+      <c r="BB9" s="47">
         <v>0.99999999999993627</v>
       </c>
-      <c r="BC9" s="52">
+      <c r="BC9" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B10" s="45">
+      <c r="B10" s="42">
         <v>6</v>
       </c>
-      <c r="C10" s="52">
+      <c r="C10" s="47">
         <f>INDEX($AB$6:$AI$14, MATCH(C13, $AA$6:$AA$14, 0), MATCH($V$10, $AB$3:$AI$3, 0))</f>
         <v>0.99999999999945333</v>
       </c>
-      <c r="D10" s="52">
+      <c r="D10" s="47">
         <f t="shared" ref="D10:H10" si="15">INDEX($AB$6:$AI$14, MATCH(D13, $AA$6:$AA$14, 0), MATCH($V$10, $AB$3:$AI$3, 0))</f>
         <v>0.99959823430951478</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="47">
         <f t="shared" si="15"/>
         <v>0.9795658771957636</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="47">
         <f t="shared" si="15"/>
         <v>0.96631005589236407</v>
       </c>
-      <c r="G10" s="52">
+      <c r="G10" s="47">
         <f t="shared" si="15"/>
         <v>0.76478079525417386</v>
       </c>
-      <c r="H10" s="52">
+      <c r="H10" s="47">
         <f t="shared" si="15"/>
         <v>0.30633564692244153</v>
       </c>
-      <c r="I10" s="52">
+      <c r="I10" s="47">
         <f>INDEX($AL$6:$AS$14, MATCH(I13, $AK$6:$AK$14, 0), MATCH($V10, $AL$3:$AS$3, 0))</f>
         <v>0.99999823974334678</v>
       </c>
-      <c r="J10" s="52">
+      <c r="J10" s="47">
         <f t="shared" ref="J10:N10" si="16">INDEX($AL$6:$AS$14, MATCH(J13, $AK$6:$AK$14, 0), MATCH($V10, $AL$3:$AS$3, 0))</f>
         <v>0.99969530786128746</v>
       </c>
-      <c r="K10" s="52">
+      <c r="K10" s="47">
         <f t="shared" si="16"/>
         <v>0.96503029194003964</v>
       </c>
-      <c r="L10" s="52">
+      <c r="L10" s="47">
         <f t="shared" si="16"/>
         <v>0.70169583060873153</v>
       </c>
-      <c r="M10" s="52">
+      <c r="M10" s="47">
         <f t="shared" si="16"/>
         <v>0.46159880109745322</v>
       </c>
-      <c r="N10" s="52">
+      <c r="N10" s="47">
         <f t="shared" si="16"/>
         <v>0.2558071850950065</v>
       </c>
-      <c r="O10" s="52">
+      <c r="O10" s="47">
         <f>INDEX($AV$6:$BC$14, MATCH(O13, $AU$6:$AU$14, 0), MATCH($V10, $AV$3:$BC$3, 0))</f>
         <v>0.99999999466107425</v>
       </c>
-      <c r="P10" s="52">
+      <c r="P10" s="47">
         <f t="shared" ref="P10:T10" si="17">INDEX($AV$6:$BC$14, MATCH(P13, $AU$6:$AU$14, 0), MATCH($V10, $AV$3:$BC$3, 0))</f>
         <v>0.99970053530100189</v>
       </c>
-      <c r="Q10" s="52">
+      <c r="Q10" s="47">
         <f t="shared" si="17"/>
         <v>0.91179733138324648</v>
       </c>
-      <c r="R10" s="52">
+      <c r="R10" s="47">
         <f t="shared" si="17"/>
         <v>0.5908714474634762</v>
       </c>
-      <c r="S10" s="52">
+      <c r="S10" s="47">
         <f t="shared" si="17"/>
         <v>0.31163257381350196</v>
       </c>
-      <c r="T10" s="52">
+      <c r="T10" s="47">
         <f t="shared" si="17"/>
         <v>8.6253363635820451E-2</v>
       </c>
@@ -9830,163 +9830,163 @@
         <v>4</v>
       </c>
       <c r="W10" s="8"/>
-      <c r="AA10" s="50" t="s">
+      <c r="AA10" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="AB10" s="52">
+      <c r="AB10" s="47">
         <v>0.5138907043261417</v>
       </c>
-      <c r="AC10" s="52">
+      <c r="AC10" s="47">
         <v>0.70275414783970647</v>
       </c>
-      <c r="AD10" s="52">
+      <c r="AD10" s="47">
         <v>0.80620969874302539</v>
       </c>
-      <c r="AE10" s="52">
+      <c r="AE10" s="47">
         <v>0.95479136080813631</v>
       </c>
-      <c r="AF10" s="52">
+      <c r="AF10" s="47">
         <v>0.99417194789886376</v>
       </c>
-      <c r="AG10" s="52">
+      <c r="AG10" s="47">
         <v>0.99959823430951478</v>
       </c>
-      <c r="AH10" s="52">
+      <c r="AH10" s="47">
         <v>0.99998547336263233</v>
       </c>
-      <c r="AI10" s="52">
+      <c r="AI10" s="47">
         <v>0</v>
       </c>
       <c r="AJ10" s="8"/>
-      <c r="AK10" s="50" t="s">
+      <c r="AK10" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="AL10" s="52">
+      <c r="AL10" s="47">
         <v>0.25380085256173046</v>
       </c>
-      <c r="AM10" s="52">
+      <c r="AM10" s="47">
         <v>0.48042786872418958</v>
       </c>
-      <c r="AN10" s="52">
+      <c r="AN10" s="47">
         <v>0.64054584703308814</v>
       </c>
-      <c r="AO10" s="52">
+      <c r="AO10" s="47">
         <v>0.91657755012121211</v>
       </c>
-      <c r="AP10" s="52">
+      <c r="AP10" s="47">
         <v>0.99191173064402915</v>
       </c>
-      <c r="AQ10" s="52">
+      <c r="AQ10" s="47">
         <v>0.99969530786128746</v>
       </c>
-      <c r="AR10" s="52">
+      <c r="AR10" s="47">
         <v>0.9999957044409139</v>
       </c>
-      <c r="AS10" s="52">
+      <c r="AS10" s="47">
         <v>0</v>
       </c>
       <c r="AT10" s="8"/>
-      <c r="AU10" s="50" t="s">
+      <c r="AU10" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="AV10" s="52">
+      <c r="AV10" s="47">
         <v>6.6011404930960929E-2</v>
       </c>
-      <c r="AW10" s="52">
+      <c r="AW10" s="47">
         <v>0.22200714259760385</v>
       </c>
-      <c r="AX10" s="52">
+      <c r="AX10" s="47">
         <v>0.39296290098211079</v>
       </c>
-      <c r="AY10" s="52">
+      <c r="AY10" s="47">
         <v>0.83221694488457221</v>
       </c>
-      <c r="AZ10" s="52">
+      <c r="AZ10" s="47">
         <v>0.98600872265415918</v>
       </c>
-      <c r="BA10" s="52">
+      <c r="BA10" s="47">
         <v>0.99970053530100189</v>
       </c>
-      <c r="BB10" s="52">
+      <c r="BB10" s="47">
         <v>0.99999846937326342</v>
       </c>
-      <c r="BC10" s="52">
+      <c r="BC10" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B11" s="45">
+      <c r="B11" s="42">
         <v>7</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="47">
         <f>INDEX($AB$6:$AI$14, MATCH(C13, $AA$6:$AA$14, 0), MATCH($V$11, $AB$3:$AI$3, 0))</f>
         <v>1</v>
       </c>
-      <c r="D11" s="52">
+      <c r="D11" s="47">
         <f t="shared" ref="D11:H11" si="18">INDEX($AB$6:$AI$14, MATCH(D13, $AA$6:$AA$14, 0), MATCH($V$11, $AB$3:$AI$3, 0))</f>
         <v>0.99998547336263233</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="47">
         <f t="shared" si="18"/>
         <v>0.99579540336422534</v>
       </c>
-      <c r="F11" s="52">
+      <c r="F11" s="47">
         <f t="shared" si="18"/>
         <v>0.99428730510778573</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="47">
         <f t="shared" si="18"/>
         <v>0.89160576223881305</v>
       </c>
-      <c r="H11" s="52">
+      <c r="H11" s="47">
         <f t="shared" si="18"/>
         <v>0.42660254978994411</v>
       </c>
-      <c r="I11" s="52">
+      <c r="I11" s="47">
         <f>INDEX($AL$6:$AS$14, MATCH(I13, $AK$6:$AK$14, 0), MATCH($V11, $AL$3:$AS$3, 0))</f>
         <v>0.99999999680227936</v>
       </c>
-      <c r="J11" s="52">
+      <c r="J11" s="47">
         <f t="shared" ref="J11:N11" si="19">INDEX($AL$6:$AS$14, MATCH(J13, $AK$6:$AK$14, 0), MATCH($V11, $AL$3:$AS$3, 0))</f>
         <v>0.9999957044409139</v>
       </c>
-      <c r="K11" s="52">
+      <c r="K11" s="47">
         <f t="shared" si="19"/>
         <v>0.99535165071760523</v>
       </c>
-      <c r="L11" s="52">
+      <c r="L11" s="47">
         <f t="shared" si="19"/>
         <v>0.85804642932382791</v>
       </c>
-      <c r="M11" s="52">
+      <c r="M11" s="47">
         <f t="shared" si="19"/>
         <v>0.63375133998904754</v>
       </c>
-      <c r="N11" s="52">
+      <c r="N11" s="47">
         <f t="shared" si="19"/>
         <v>0.362347970092745</v>
       </c>
-      <c r="O11" s="52">
+      <c r="O11" s="47">
         <f>INDEX($AV$6:$BC$14, MATCH(O13, $AU$6:$AU$14, 0), MATCH($V11, $AV$3:$BC$3, 0))</f>
         <v>0.99999999999993627</v>
       </c>
-      <c r="P11" s="52">
+      <c r="P11" s="47">
         <f t="shared" ref="P11:T11" si="20">INDEX($AV$6:$BC$14, MATCH(P13, $AU$6:$AU$14, 0), MATCH($V11, $AV$3:$BC$3, 0))</f>
         <v>0.99999846937326342</v>
       </c>
-      <c r="Q11" s="52">
+      <c r="Q11" s="47">
         <f t="shared" si="20"/>
         <v>0.98146734609448394</v>
       </c>
-      <c r="R11" s="52">
+      <c r="R11" s="47">
         <f t="shared" si="20"/>
         <v>0.77688109740361544</v>
       </c>
-      <c r="S11" s="52">
+      <c r="S11" s="47">
         <f t="shared" si="20"/>
         <v>0.49844467341211474</v>
       </c>
-      <c r="T11" s="52">
+      <c r="T11" s="47">
         <f t="shared" si="20"/>
         <v>0.15295879709707286</v>
       </c>
@@ -9995,173 +9995,173 @@
         <v>4.5</v>
       </c>
       <c r="W11" s="8"/>
-      <c r="AA11" s="49" t="s">
+      <c r="AA11" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="AB11" s="52">
+      <c r="AB11" s="47">
         <v>0.37584533679027893</v>
       </c>
-      <c r="AC11" s="52">
+      <c r="AC11" s="47">
         <v>0.51506861469064869</v>
       </c>
-      <c r="AD11" s="52">
+      <c r="AD11" s="47">
         <v>0.60792230376456446</v>
       </c>
-      <c r="AE11" s="52">
+      <c r="AE11" s="47">
         <v>0.80626831138166599</v>
       </c>
-      <c r="AF11" s="52">
+      <c r="AF11" s="47">
         <v>0.92710242952401201</v>
       </c>
-      <c r="AG11" s="52">
+      <c r="AG11" s="47">
         <v>0.9795658771957636</v>
       </c>
-      <c r="AH11" s="52">
+      <c r="AH11" s="47">
         <v>0.99579540336422534</v>
       </c>
-      <c r="AI11" s="52">
+      <c r="AI11" s="47">
         <v>0</v>
       </c>
       <c r="AJ11" s="8"/>
-      <c r="AK11" s="49" t="s">
+      <c r="AK11" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="AL11" s="52">
+      <c r="AL11" s="47">
         <v>8.9754023843298891E-2</v>
       </c>
-      <c r="AM11" s="52">
+      <c r="AM11" s="47">
         <v>0.19240027281705166</v>
       </c>
-      <c r="AN11" s="52">
+      <c r="AN11" s="47">
         <v>0.28991681177663592</v>
       </c>
-      <c r="AO11" s="52">
+      <c r="AO11" s="47">
         <v>0.59290175446950721</v>
       </c>
-      <c r="AP11" s="52">
+      <c r="AP11" s="47">
         <v>0.8470018886690438</v>
       </c>
-      <c r="AQ11" s="52">
+      <c r="AQ11" s="47">
         <v>0.96503029194003964</v>
       </c>
-      <c r="AR11" s="52">
+      <c r="AR11" s="47">
         <v>0.99535165071760523</v>
       </c>
-      <c r="AS11" s="52">
+      <c r="AS11" s="47">
         <v>0</v>
       </c>
       <c r="AT11" s="8"/>
-      <c r="AU11" s="49" t="s">
+      <c r="AU11" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="AV11" s="52">
+      <c r="AV11" s="47">
         <v>5.6979596817344061E-2</v>
       </c>
-      <c r="AW11" s="52">
+      <c r="AW11" s="47">
         <v>0.12698439253107691</v>
       </c>
-      <c r="AX11" s="52">
+      <c r="AX11" s="47">
         <v>0.19835620119859471</v>
       </c>
-      <c r="AY11" s="52">
+      <c r="AY11" s="47">
         <v>0.45447244481580307</v>
       </c>
-      <c r="AZ11" s="52">
+      <c r="AZ11" s="47">
         <v>0.73196550526672355</v>
       </c>
-      <c r="BA11" s="52">
+      <c r="BA11" s="47">
         <v>0.91179733138324648</v>
       </c>
-      <c r="BB11" s="52">
+      <c r="BB11" s="47">
         <v>0.98146734609448394</v>
       </c>
-      <c r="BC11" s="52">
+      <c r="BC11" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="AA12" s="50" t="s">
+      <c r="AA12" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="AB12" s="52">
+      <c r="AB12" s="47">
         <v>0.16552806134367962</v>
       </c>
-      <c r="AC12" s="52">
+      <c r="AC12" s="47">
         <v>0.29053559209062707</v>
       </c>
-      <c r="AD12" s="52">
+      <c r="AD12" s="47">
         <v>0.39292301197938029</v>
       </c>
-      <c r="AE12" s="52">
+      <c r="AE12" s="47">
         <v>0.66588242910237538</v>
       </c>
-      <c r="AF12" s="52">
+      <c r="AF12" s="47">
         <v>0.87051976694100974</v>
       </c>
-      <c r="AG12" s="52">
+      <c r="AG12" s="47">
         <v>0.96631005589236407</v>
       </c>
-      <c r="AH12" s="52">
+      <c r="AH12" s="47">
         <v>0.99428730510778573</v>
       </c>
-      <c r="AI12" s="52">
+      <c r="AI12" s="47">
         <v>0</v>
       </c>
       <c r="AJ12" s="8"/>
-      <c r="AK12" s="50" t="s">
+      <c r="AK12" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="AL12" s="52">
+      <c r="AL12" s="47">
         <v>5.0511604601422351E-2</v>
       </c>
-      <c r="AM12" s="52">
+      <c r="AM12" s="47">
         <v>9.4333345509310967E-2</v>
       </c>
-      <c r="AN12" s="52">
+      <c r="AN12" s="47">
         <v>0.13618656405660809</v>
       </c>
-      <c r="AO12" s="52">
+      <c r="AO12" s="47">
         <v>0.28933976981199794</v>
       </c>
-      <c r="AP12" s="52">
+      <c r="AP12" s="47">
         <v>0.49480783925100147</v>
       </c>
-      <c r="AQ12" s="52">
+      <c r="AQ12" s="47">
         <v>0.70169583060873153</v>
       </c>
-      <c r="AR12" s="52">
+      <c r="AR12" s="47">
         <v>0.85804642932382791</v>
       </c>
-      <c r="AS12" s="52">
+      <c r="AS12" s="47">
         <v>0</v>
       </c>
       <c r="AT12" s="8"/>
-      <c r="AU12" s="50" t="s">
+      <c r="AU12" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="AV12" s="52">
+      <c r="AV12" s="47">
         <v>2.8856450394145666E-2</v>
       </c>
-      <c r="AW12" s="52">
+      <c r="AW12" s="47">
         <v>5.7199757058308189E-2</v>
       </c>
-      <c r="AX12" s="52">
+      <c r="AX12" s="47">
         <v>8.5976160021217857E-2</v>
       </c>
-      <c r="AY12" s="52">
+      <c r="AY12" s="47">
         <v>0.20212850255165354</v>
       </c>
-      <c r="AZ12" s="52">
+      <c r="AZ12" s="47">
         <v>0.38127737390844418</v>
       </c>
-      <c r="BA12" s="52">
+      <c r="BA12" s="47">
         <v>0.5908714474634762</v>
       </c>
-      <c r="BB12" s="52">
+      <c r="BB12" s="47">
         <v>0.77688109740361544</v>
       </c>
-      <c r="BC12" s="52">
+      <c r="BC12" s="47">
         <v>0</v>
       </c>
     </row>
@@ -10223,174 +10223,174 @@
       <c r="T13" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="AA13" s="49" t="s">
+      <c r="AA13" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="AB13" s="52">
+      <c r="AB13" s="47">
         <v>9.1492186931267622E-2</v>
       </c>
-      <c r="AC13" s="52">
+      <c r="AC13" s="47">
         <v>0.15300882371326033</v>
       </c>
-      <c r="AD13" s="52">
+      <c r="AD13" s="47">
         <v>0.20660004501142309</v>
       </c>
-      <c r="AE13" s="52">
+      <c r="AE13" s="47">
         <v>0.38021044483571315</v>
       </c>
-      <c r="AF13" s="52">
+      <c r="AF13" s="47">
         <v>0.58254904641534866</v>
       </c>
-      <c r="AG13" s="52">
+      <c r="AG13" s="47">
         <v>0.76478079525417386</v>
       </c>
-      <c r="AH13" s="52">
+      <c r="AH13" s="47">
         <v>0.89160576223881305</v>
       </c>
-      <c r="AI13" s="52">
+      <c r="AI13" s="47">
         <v>0</v>
       </c>
       <c r="AJ13" s="8"/>
-      <c r="AK13" s="49" t="s">
+      <c r="AK13" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="AL13" s="52">
+      <c r="AL13" s="47">
         <v>3.2210497290905374E-2</v>
       </c>
-      <c r="AM13" s="52">
+      <c r="AM13" s="47">
         <v>5.6332486553475364E-2</v>
       </c>
-      <c r="AN13" s="52">
+      <c r="AN13" s="47">
         <v>7.9115975834815E-2</v>
       </c>
-      <c r="AO13" s="52">
+      <c r="AO13" s="47">
         <v>0.16531868864588461</v>
       </c>
-      <c r="AP13" s="52">
+      <c r="AP13" s="47">
         <v>0.29645675583092174</v>
       </c>
-      <c r="AQ13" s="52">
+      <c r="AQ13" s="47">
         <v>0.46159880109745322</v>
       </c>
-      <c r="AR13" s="52">
+      <c r="AR13" s="47">
         <v>0.63375133998904754</v>
       </c>
-      <c r="AS13" s="52">
+      <c r="AS13" s="47">
         <v>0</v>
       </c>
       <c r="AT13" s="8"/>
-      <c r="AU13" s="49" t="s">
+      <c r="AU13" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="AV13" s="52">
+      <c r="AV13" s="47">
         <v>7.3325429420576533E-3</v>
       </c>
-      <c r="AW13" s="52">
+      <c r="AW13" s="47">
         <v>1.5850994164039133E-2</v>
       </c>
-      <c r="AX13" s="52">
+      <c r="AX13" s="47">
         <v>2.5396980814932565E-2</v>
       </c>
-      <c r="AY13" s="52">
+      <c r="AY13" s="47">
         <v>7.1339545297204487E-2</v>
       </c>
-      <c r="AZ13" s="52">
+      <c r="AZ13" s="47">
         <v>0.16389933245411942</v>
       </c>
-      <c r="BA13" s="52">
+      <c r="BA13" s="47">
         <v>0.31163257381350196</v>
       </c>
-      <c r="BB13" s="52">
+      <c r="BB13" s="47">
         <v>0.49844467341211474</v>
       </c>
-      <c r="BC13" s="52">
+      <c r="BC13" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="AA14" s="51" t="s">
+      <c r="AA14" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="AB14" s="52">
+      <c r="AB14" s="47">
         <v>3.6630747396996691E-2</v>
       </c>
-      <c r="AC14" s="52">
+      <c r="AC14" s="47">
         <v>5.4970533940220757E-2</v>
       </c>
-      <c r="AD14" s="52">
+      <c r="AD14" s="47">
         <v>7.0785662206478708E-2</v>
       </c>
-      <c r="AE14" s="52">
+      <c r="AE14" s="47">
         <v>0.12533343317165579</v>
       </c>
-      <c r="AF14" s="52">
+      <c r="AF14" s="47">
         <v>0.20397754353748057</v>
       </c>
-      <c r="AG14" s="52">
+      <c r="AG14" s="47">
         <v>0.30633564692244153</v>
       </c>
-      <c r="AH14" s="52">
+      <c r="AH14" s="47">
         <v>0.42660254978994411</v>
       </c>
-      <c r="AI14" s="52">
+      <c r="AI14" s="47">
         <v>0</v>
       </c>
       <c r="AJ14" s="8"/>
-      <c r="AK14" s="51" t="s">
+      <c r="AK14" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="AL14" s="52">
+      <c r="AL14" s="47">
         <v>3.054309712927282E-2</v>
       </c>
-      <c r="AM14" s="52">
+      <c r="AM14" s="47">
         <v>4.54767509141593E-2</v>
       </c>
-      <c r="AN14" s="52">
+      <c r="AN14" s="47">
         <v>5.8354873920238394E-2</v>
       </c>
-      <c r="AO14" s="52">
+      <c r="AO14" s="47">
         <v>0.10300763832828137</v>
       </c>
-      <c r="AP14" s="52">
+      <c r="AP14" s="47">
         <v>0.16841130134712209</v>
       </c>
-      <c r="AQ14" s="52">
+      <c r="AQ14" s="47">
         <v>0.2558071850950065</v>
       </c>
-      <c r="AR14" s="52">
+      <c r="AR14" s="47">
         <v>0.362347970092745</v>
       </c>
-      <c r="AS14" s="52">
+      <c r="AS14" s="47">
         <v>0</v>
       </c>
       <c r="AT14" s="8"/>
-      <c r="AU14" s="51" t="s">
+      <c r="AU14" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="AV14" s="52">
+      <c r="AV14" s="47">
         <v>3.2086171243230267E-3</v>
       </c>
-      <c r="AW14" s="52">
+      <c r="AW14" s="47">
         <v>5.8437278169573741E-3</v>
       </c>
-      <c r="AX14" s="52">
+      <c r="AX14" s="47">
         <v>8.5326893308700167E-3</v>
       </c>
-      <c r="AY14" s="52">
+      <c r="AY14" s="47">
         <v>2.0430952713542849E-2</v>
       </c>
-      <c r="AZ14" s="52">
+      <c r="AZ14" s="47">
         <v>4.4138172035112347E-2</v>
       </c>
-      <c r="BA14" s="52">
+      <c r="BA14" s="47">
         <v>8.6253363635820451E-2</v>
       </c>
-      <c r="BB14" s="52">
+      <c r="BB14" s="47">
         <v>0.15295879709707286</v>
       </c>
-      <c r="BC14" s="52">
+      <c r="BC14" s="47">
         <v>0</v>
       </c>
     </row>
@@ -10498,11 +10498,12 @@
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="35">
+        <f>O19</f>
         <v>0.76682617615099935</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
-      <c r="O19" s="53">
+      <c r="O19" s="48">
         <f>INDEX($C$5:$T$11, MATCH($A$2, $B$5:$B$11, 0), MATCH(E19, $C$4:$T$4, 0))</f>
         <v>0.76682617615099935</v>
       </c>
@@ -10525,11 +10526,12 @@
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="35">
+        <f t="shared" ref="K20:K24" si="21">O20</f>
         <v>0.5138907043261417</v>
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
-      <c r="O20" s="53">
+      <c r="O20" s="48">
         <f>INDEX($C$5:$T$11, MATCH($A$2, $B$5:$B$11, 0), MATCH(E20, $C$4:$T$4, 0))</f>
         <v>0.5138907043261417</v>
       </c>
@@ -10552,12 +10554,13 @@
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="35">
+        <f t="shared" si="21"/>
         <v>0.37584533679027893</v>
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
-      <c r="O21" s="53">
-        <f t="shared" ref="O21:O25" si="21">INDEX($C$5:$T$11, MATCH($A$2, $B$5:$B$11, 0), MATCH(E21, $C$4:$T$4, 0))</f>
+      <c r="O21" s="48">
+        <f t="shared" ref="O21:O24" si="22">INDEX($C$5:$T$11, MATCH($A$2, $B$5:$B$11, 0), MATCH(E21, $C$4:$T$4, 0))</f>
         <v>0.37584533679027893</v>
       </c>
       <c r="P21" s="8"/>
@@ -10579,12 +10582,13 @@
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="35">
+        <f t="shared" si="21"/>
         <v>0.16552806134367962</v>
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
-      <c r="O22" s="53">
-        <f t="shared" si="21"/>
+      <c r="O22" s="48">
+        <f t="shared" si="22"/>
         <v>0.16552806134367962</v>
       </c>
       <c r="P22" s="8"/>
@@ -10606,12 +10610,13 @@
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="35">
+        <f t="shared" si="21"/>
         <v>9.1492186931267622E-2</v>
       </c>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
-      <c r="O23" s="53">
-        <f t="shared" si="21"/>
+      <c r="O23" s="48">
+        <f t="shared" si="22"/>
         <v>9.1492186931267622E-2</v>
       </c>
       <c r="P23" s="8"/>
@@ -10633,12 +10638,13 @@
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="35">
+        <f t="shared" si="21"/>
         <v>3.6630747396996691E-2</v>
       </c>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
-      <c r="O24" s="53">
-        <f t="shared" si="21"/>
+      <c r="O24" s="48">
+        <f t="shared" si="22"/>
         <v>3.6630747396996691E-2</v>
       </c>
       <c r="P24" s="8"/>
@@ -10738,11 +10744,12 @@
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="35">
+        <f>O28</f>
         <v>0.48602123970467664</v>
       </c>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
-      <c r="O28" s="53">
+      <c r="O28" s="48">
         <f>INDEX($C$5:$T$11, MATCH($A$2, $B$5:$B$11, 0), MATCH(E28, $C$4:$T$4, 0))</f>
         <v>0.48602123970467664</v>
       </c>
@@ -10765,12 +10772,13 @@
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="35">
+        <f t="shared" ref="K29:K33" si="23">O29</f>
         <v>0.25380085256173046</v>
       </c>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
-      <c r="O29" s="53">
-        <f t="shared" ref="O29:O33" si="22">INDEX($C$5:$T$11, MATCH($A$2, $B$5:$B$11, 0), MATCH(E29, $C$4:$T$4, 0))</f>
+      <c r="O29" s="48">
+        <f t="shared" ref="O29:O33" si="24">INDEX($C$5:$T$11, MATCH($A$2, $B$5:$B$11, 0), MATCH(E29, $C$4:$T$4, 0))</f>
         <v>0.25380085256173046</v>
       </c>
       <c r="P29" s="8"/>
@@ -10792,12 +10800,13 @@
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="35">
+        <f t="shared" si="23"/>
         <v>8.9754023843298891E-2</v>
       </c>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
-      <c r="O30" s="53">
-        <f t="shared" si="22"/>
+      <c r="O30" s="48">
+        <f t="shared" si="24"/>
         <v>8.9754023843298891E-2</v>
       </c>
       <c r="P30" s="8"/>
@@ -10819,12 +10828,13 @@
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="35">
+        <f t="shared" si="23"/>
         <v>5.0511604601422351E-2</v>
       </c>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
-      <c r="O31" s="53">
-        <f t="shared" si="22"/>
+      <c r="O31" s="48">
+        <f t="shared" si="24"/>
         <v>5.0511604601422351E-2</v>
       </c>
       <c r="P31" s="8"/>
@@ -10846,12 +10856,13 @@
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="35">
+        <f t="shared" si="23"/>
         <v>3.2210497290905374E-2</v>
       </c>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
-      <c r="O32" s="53">
-        <f t="shared" si="22"/>
+      <c r="O32" s="48">
+        <f t="shared" si="24"/>
         <v>3.2210497290905374E-2</v>
       </c>
       <c r="P32" s="8"/>
@@ -10873,12 +10884,13 @@
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="35">
+        <f t="shared" si="23"/>
         <v>3.054309712927282E-2</v>
       </c>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
-      <c r="O33" s="53">
-        <f t="shared" si="22"/>
+      <c r="O33" s="48">
+        <f t="shared" si="24"/>
         <v>3.054309712927282E-2</v>
       </c>
       <c r="P33" s="8"/>
@@ -10976,11 +10988,12 @@
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="35">
+        <f>O37</f>
         <v>0.14983014442834014</v>
       </c>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
-      <c r="O37" s="53">
+      <c r="O37" s="48">
         <f>INDEX($C$5:$T$11, MATCH($A$2, $B$5:$B$11, 0), MATCH(E37, $C$4:$T$4, 0))</f>
         <v>0.14983014442834014</v>
       </c>
@@ -11003,12 +11016,13 @@
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="35">
+        <f t="shared" ref="K38:K42" si="25">O38</f>
         <v>6.6011404930960929E-2</v>
       </c>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
-      <c r="O38" s="53">
-        <f t="shared" ref="O38:O42" si="23">INDEX($C$5:$T$11, MATCH($A$2, $B$5:$B$11, 0), MATCH(E38, $C$4:$T$4, 0))</f>
+      <c r="O38" s="48">
+        <f t="shared" ref="O38:O42" si="26">INDEX($C$5:$T$11, MATCH($A$2, $B$5:$B$11, 0), MATCH(E38, $C$4:$T$4, 0))</f>
         <v>6.6011404930960929E-2</v>
       </c>
       <c r="P38" s="8"/>
@@ -11030,12 +11044,13 @@
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="35">
+        <f t="shared" si="25"/>
         <v>5.6979596817344061E-2</v>
       </c>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
-      <c r="O39" s="53">
-        <f t="shared" si="23"/>
+      <c r="O39" s="48">
+        <f t="shared" si="26"/>
         <v>5.6979596817344061E-2</v>
       </c>
       <c r="P39" s="8"/>
@@ -11057,12 +11072,13 @@
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="35">
+        <f t="shared" si="25"/>
         <v>2.8856450394145666E-2</v>
       </c>
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
-      <c r="O40" s="53">
-        <f t="shared" si="23"/>
+      <c r="O40" s="48">
+        <f t="shared" si="26"/>
         <v>2.8856450394145666E-2</v>
       </c>
       <c r="P40" s="8"/>
@@ -11084,12 +11100,13 @@
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="35">
+        <f t="shared" si="25"/>
         <v>7.3325429420576533E-3</v>
       </c>
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
-      <c r="O41" s="53">
-        <f t="shared" si="23"/>
+      <c r="O41" s="48">
+        <f t="shared" si="26"/>
         <v>7.3325429420576533E-3</v>
       </c>
       <c r="P41" s="8"/>
@@ -11111,12 +11128,13 @@
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="35">
+        <f t="shared" si="25"/>
         <v>3.2086171243230267E-3</v>
       </c>
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
-      <c r="O42" s="53">
-        <f t="shared" si="23"/>
+      <c r="O42" s="48">
+        <f t="shared" si="26"/>
         <v>3.2086171243230267E-3</v>
       </c>
     </row>

</xml_diff>